<commit_message>
Add validation error code049 to sampling and isolation date.
Ticket: #118
Change-Id: Ic58c5a178a8f9602d78c6fd8dbf5c00f9c60b0dd
</commit_message>
<xml_diff>
--- a/testData/MiBi-TEST_Probenummer-AVVData-Erreger_mps67_Error-3-5-6-10-49-68,69,73,95.xlsx
+++ b/testData/MiBi-TEST_Probenummer-AVVData-Erreger_mps67_Error-3-5-6-10-49-68,69,73,95.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="277">
   <si>
     <r>
       <rPr>
@@ -727,25 +727,6 @@
     <t xml:space="preserve">8</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">68,95,6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">,72</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">126</t>
   </si>
   <si>
@@ -794,23 +775,7 @@
     <t xml:space="preserve">ERROR: If  Probenummer  is not given, identical Probenummer nach AVVData with identical Erreger always result in an error, regardless of the reason (lines 13+14)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">68,6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">,72</t>
-    </r>
+    <t xml:space="preserve">68,6,72</t>
   </si>
   <si>
     <t xml:space="preserve">14</t>
@@ -825,23 +790,7 @@
     <t xml:space="preserve">ERROR: Erreger must always be given, otherwise no NRL at BfR will analyse the sample</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">10,95</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">,72</t>
-    </r>
+    <t xml:space="preserve">10,95,72</t>
   </si>
   <si>
     <t xml:space="preserve">130</t>
@@ -874,7 +823,7 @@
     <t xml:space="preserve">NOT SH6; ERROR: No Probenummer AVVData AND Grund der Probenahme = ZoMo; Attention: First check combination of year+ADV2+3+8+16 whether it really is a ZoMo sample; if yes: ERROR  AVVData is missing; if not: ERROR Grund der Probenahme is erroneous and must be corrected</t>
   </si>
   <si>
-    <t xml:space="preserve">5,49,49,49,49</t>
+    <t xml:space="preserve">5,49,49,49,49,49,49</t>
   </si>
   <si>
     <t xml:space="preserve">133</t>
@@ -892,23 +841,7 @@
     <t xml:space="preserve">ERROR: Duplicate Probenummer AVVData AND Erreger (lines 20+21)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">95,3,6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">,72</t>
-    </r>
+    <t xml:space="preserve">95,3,6,72</t>
   </si>
   <si>
     <t xml:space="preserve">Hinweise zum Einsendeformular des BfR:</t>
@@ -2279,7 +2212,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="MM/DD/YYYY"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2436,11 +2369,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -3446,43 +3374,43 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="4" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="4" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3538,7 +3466,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3594,11 +3522,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="11" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="11" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3614,7 +3542,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="28" fillId="11" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="27" fillId="11" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3634,11 +3562,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="11" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="11" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="11" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="11" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3646,11 +3574,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3658,7 +3586,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3670,7 +3598,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="11" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="11" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3686,7 +3614,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="28" fillId="11" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="27" fillId="11" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3698,11 +3626,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3714,11 +3642,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3726,7 +3654,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3738,7 +3666,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3925,9 +3853,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>1703160</xdr:colOff>
+      <xdr:colOff>1702800</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3940,8 +3868,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12320280" y="57240"/>
-          <a:ext cx="1699200" cy="618480"/>
+          <a:off x="12319560" y="57240"/>
+          <a:ext cx="1698840" cy="618120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3964,7 +3892,7 @@
   <dimension ref="A1:Y67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K59" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S62" activeCellId="0" sqref="S62"/>
+      <selection pane="topLeft" activeCell="S60" activeCellId="0" sqref="S60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3973,7 +3901,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.99"/>
@@ -5417,19 +5345,19 @@
         <v>102</v>
       </c>
       <c r="S49" s="69" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" s="69" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="72" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B50" s="64"/>
       <c r="C50" s="64" t="s">
         <v>71</v>
       </c>
       <c r="D50" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E50" s="65" t="n">
         <v>43102</v>
@@ -5463,15 +5391,15 @@
       </c>
       <c r="Q50" s="64"/>
       <c r="R50" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="S50" s="69" t="s">
         <v>108</v>
-      </c>
-      <c r="S50" s="69" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="51" s="69" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="72" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B51" s="64"/>
       <c r="C51" s="64" t="s">
@@ -5512,22 +5440,22 @@
       </c>
       <c r="Q51" s="64"/>
       <c r="R51" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="S51" s="69" t="s">
         <v>108</v>
-      </c>
-      <c r="S51" s="69" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="52" s="69" customFormat="true" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B52" s="63"/>
       <c r="C52" s="64" t="s">
         <v>71</v>
       </c>
       <c r="D52" s="64" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E52" s="65" t="n">
         <v>43102</v>
@@ -5546,22 +5474,22 @@
         <v>75</v>
       </c>
       <c r="K52" s="64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L52" s="64"/>
       <c r="M52" s="64" t="s">
         <v>77</v>
       </c>
       <c r="N52" s="64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O52" s="64"/>
       <c r="P52" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q52" s="64"/>
       <c r="R52" s="66" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S52" s="69" t="n">
         <v>5</v>
@@ -5569,14 +5497,14 @@
     </row>
     <row r="53" s="69" customFormat="true" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B53" s="63"/>
       <c r="C53" s="64" t="s">
         <v>71</v>
       </c>
       <c r="D53" s="64" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E53" s="65" t="n">
         <v>43102</v>
@@ -5595,7 +5523,7 @@
         <v>75</v>
       </c>
       <c r="K53" s="64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L53" s="64"/>
       <c r="M53" s="64" t="s">
@@ -5603,14 +5531,14 @@
       </c>
       <c r="N53" s="64"/>
       <c r="O53" s="64" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P53" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q53" s="64"/>
       <c r="R53" s="66" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S53" s="69" t="n">
         <v>5</v>
@@ -5619,13 +5547,13 @@
     <row r="54" s="69" customFormat="true" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="64"/>
       <c r="B54" s="73" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C54" s="64" t="s">
         <v>71</v>
       </c>
       <c r="D54" s="64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E54" s="65" t="n">
         <v>43102</v>
@@ -5644,37 +5572,37 @@
         <v>75</v>
       </c>
       <c r="K54" s="64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L54" s="64"/>
       <c r="M54" s="64" t="s">
         <v>77</v>
       </c>
       <c r="N54" s="64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O54" s="64"/>
       <c r="P54" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q54" s="74"/>
       <c r="R54" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="S54" s="69" t="s">
         <v>121</v>
-      </c>
-      <c r="S54" s="69" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="55" s="75" customFormat="true" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="64"/>
       <c r="B55" s="73" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C55" s="64" t="s">
         <v>71</v>
       </c>
       <c r="D55" s="64" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E55" s="65" t="n">
         <v>43102</v>
@@ -5693,7 +5621,7 @@
         <v>75</v>
       </c>
       <c r="K55" s="64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L55" s="64"/>
       <c r="M55" s="64" t="s">
@@ -5701,25 +5629,25 @@
       </c>
       <c r="N55" s="64"/>
       <c r="O55" s="64" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P55" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q55" s="64"/>
       <c r="R55" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="S55" s="75" t="s">
         <v>121</v>
-      </c>
-      <c r="S55" s="75" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="56" s="75" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56" s="64" t="s">
         <v>124</v>
-      </c>
-      <c r="B56" s="64" t="s">
-        <v>125</v>
       </c>
       <c r="C56" s="63"/>
       <c r="D56" s="64" t="s">
@@ -5757,22 +5685,22 @@
       </c>
       <c r="Q56" s="64"/>
       <c r="R56" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="S56" s="75" t="s">
         <v>126</v>
-      </c>
-      <c r="S56" s="75" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="57" s="75" customFormat="true" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B57" s="63"/>
       <c r="C57" s="64" t="s">
         <v>71</v>
       </c>
       <c r="D57" s="64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E57" s="65" t="n">
         <v>43102</v>
@@ -5791,22 +5719,22 @@
         <v>75</v>
       </c>
       <c r="K57" s="64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L57" s="64"/>
       <c r="M57" s="64" t="s">
         <v>77</v>
       </c>
       <c r="N57" s="64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O57" s="64"/>
       <c r="P57" s="64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q57" s="64"/>
       <c r="R57" s="66" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S57" s="75" t="n">
         <v>5</v>
@@ -5814,14 +5742,14 @@
     </row>
     <row r="58" s="75" customFormat="true" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B58" s="63"/>
       <c r="C58" s="64" t="s">
         <v>71</v>
       </c>
       <c r="D58" s="64" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E58" s="65" t="n">
         <v>43102</v>
@@ -5840,7 +5768,7 @@
         <v>75</v>
       </c>
       <c r="K58" s="64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L58" s="64"/>
       <c r="M58" s="64" t="s">
@@ -5848,14 +5776,14 @@
       </c>
       <c r="N58" s="64"/>
       <c r="O58" s="64" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P58" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q58" s="64"/>
       <c r="R58" s="66" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S58" s="75" t="n">
         <v>5</v>
@@ -5863,14 +5791,14 @@
     </row>
     <row r="59" s="75" customFormat="true" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="64" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B59" s="63"/>
       <c r="C59" s="64" t="s">
         <v>71</v>
       </c>
       <c r="D59" s="64" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E59" s="65" t="n">
         <v>43102</v>
@@ -5886,40 +5814,40 @@
         <v>74</v>
       </c>
       <c r="J59" s="64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K59" s="64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L59" s="64"/>
       <c r="M59" s="64" t="s">
         <v>77</v>
       </c>
       <c r="N59" s="77" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O59" s="64"/>
       <c r="P59" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q59" s="64"/>
       <c r="R59" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="S59" s="75" t="s">
         <v>137</v>
-      </c>
-      <c r="S59" s="75" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="60" s="67" customFormat="true" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B60" s="63"/>
       <c r="C60" s="64" t="s">
         <v>71</v>
       </c>
       <c r="D60" s="64" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E60" s="65" t="n">
         <v>43102</v>
@@ -5935,10 +5863,10 @@
         <v>74</v>
       </c>
       <c r="J60" s="64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K60" s="64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L60" s="64"/>
       <c r="M60" s="64" t="s">
@@ -5946,25 +5874,25 @@
       </c>
       <c r="N60" s="64"/>
       <c r="O60" s="77" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P60" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q60" s="64"/>
       <c r="R60" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="S60" s="67" t="s">
         <v>137</v>
-      </c>
-      <c r="S60" s="67" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="61" s="67" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="B61" s="78" t="s">
         <v>141</v>
-      </c>
-      <c r="B61" s="78" t="s">
-        <v>142</v>
       </c>
       <c r="C61" s="78" t="s">
         <v>71</v>
@@ -6002,18 +5930,18 @@
       </c>
       <c r="Q61" s="76"/>
       <c r="R61" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="S61" s="67" t="s">
         <v>143</v>
-      </c>
-      <c r="S61" s="67" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="62" s="67" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="78" t="s">
         <v>141</v>
-      </c>
-      <c r="B62" s="78" t="s">
-        <v>142</v>
       </c>
       <c r="C62" s="78" t="s">
         <v>71</v>
@@ -6051,10 +5979,10 @@
       </c>
       <c r="Q62" s="76"/>
       <c r="R62" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="S62" s="67" t="s">
         <v>143</v>
-      </c>
-      <c r="S62" s="67" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7293,7 +7221,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="80" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -7339,7 +7267,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="82" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" s="81"/>
       <c r="C3" s="81"/>
@@ -7363,15 +7291,15 @@
     </row>
     <row r="4" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="83" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="84" t="s">
         <v>147</v>
-      </c>
-      <c r="B4" s="84" t="s">
-        <v>148</v>
       </c>
       <c r="C4" s="84"/>
       <c r="D4" s="84"/>
       <c r="E4" s="84" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F4" s="84"/>
       <c r="G4" s="84"/>
@@ -7385,25 +7313,25 @@
       <c r="O4" s="84"/>
       <c r="P4" s="84"/>
       <c r="Q4" s="85" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R4" s="85"/>
       <c r="S4" s="86" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="T4" s="86"/>
     </row>
     <row r="5" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="87" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="88" t="s">
         <v>152</v>
-      </c>
-      <c r="B5" s="88" t="s">
-        <v>153</v>
       </c>
       <c r="C5" s="88"/>
       <c r="D5" s="88"/>
       <c r="E5" s="89" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="89"/>
       <c r="G5" s="89"/>
@@ -7417,25 +7345,25 @@
       <c r="O5" s="89"/>
       <c r="P5" s="89"/>
       <c r="Q5" s="90" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R5" s="90"/>
       <c r="S5" s="91" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T5" s="91"/>
     </row>
     <row r="6" customFormat="false" ht="33.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="93" t="s">
         <v>156</v>
-      </c>
-      <c r="B6" s="93" t="s">
-        <v>157</v>
       </c>
       <c r="C6" s="93"/>
       <c r="D6" s="93"/>
       <c r="E6" s="94" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F6" s="94"/>
       <c r="G6" s="94"/>
@@ -7451,21 +7379,21 @@
       <c r="Q6" s="95"/>
       <c r="R6" s="95"/>
       <c r="S6" s="96" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T6" s="96"/>
     </row>
     <row r="7" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="92" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="93" t="s">
         <v>159</v>
-      </c>
-      <c r="B7" s="93" t="s">
-        <v>160</v>
       </c>
       <c r="C7" s="93"/>
       <c r="D7" s="93"/>
       <c r="E7" s="94" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F7" s="94"/>
       <c r="G7" s="94"/>
@@ -7479,25 +7407,25 @@
       <c r="O7" s="94"/>
       <c r="P7" s="94"/>
       <c r="Q7" s="95" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R7" s="95"/>
       <c r="S7" s="97" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T7" s="97"/>
     </row>
     <row r="8" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="92" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="93" t="s">
         <v>163</v>
-      </c>
-      <c r="B8" s="93" t="s">
-        <v>164</v>
       </c>
       <c r="C8" s="93"/>
       <c r="D8" s="93"/>
       <c r="E8" s="94" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F8" s="94"/>
       <c r="G8" s="94"/>
@@ -7517,15 +7445,15 @@
     </row>
     <row r="9" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="92" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="93" t="s">
         <v>166</v>
-      </c>
-      <c r="B9" s="93" t="s">
-        <v>167</v>
       </c>
       <c r="C9" s="93"/>
       <c r="D9" s="93"/>
       <c r="E9" s="94" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F9" s="94"/>
       <c r="G9" s="94"/>
@@ -7539,17 +7467,17 @@
       <c r="O9" s="94"/>
       <c r="P9" s="94"/>
       <c r="Q9" s="95" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R9" s="95"/>
       <c r="S9" s="97" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T9" s="97"/>
     </row>
     <row r="10" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="92" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B10" s="93" t="s">
         <v>57</v>
@@ -7557,7 +7485,7 @@
       <c r="C10" s="93"/>
       <c r="D10" s="93"/>
       <c r="E10" s="94" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F10" s="94"/>
       <c r="G10" s="94"/>
@@ -7573,21 +7501,21 @@
       <c r="Q10" s="95"/>
       <c r="R10" s="95"/>
       <c r="S10" s="97" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T10" s="97"/>
     </row>
     <row r="11" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="92" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="93" t="s">
         <v>171</v>
-      </c>
-      <c r="B11" s="93" t="s">
-        <v>172</v>
       </c>
       <c r="C11" s="93"/>
       <c r="D11" s="93"/>
       <c r="E11" s="94" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F11" s="94"/>
       <c r="G11" s="94"/>
@@ -7603,21 +7531,21 @@
       <c r="Q11" s="95"/>
       <c r="R11" s="95"/>
       <c r="S11" s="97" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T11" s="97"/>
     </row>
     <row r="12" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="92" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="93" t="s">
         <v>175</v>
-      </c>
-      <c r="B12" s="93" t="s">
-        <v>176</v>
       </c>
       <c r="C12" s="93"/>
       <c r="D12" s="93"/>
       <c r="E12" s="94" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F12" s="94"/>
       <c r="G12" s="94"/>
@@ -7637,15 +7565,15 @@
     </row>
     <row r="13" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13" s="93" t="s">
         <v>178</v>
-      </c>
-      <c r="B13" s="93" t="s">
-        <v>179</v>
       </c>
       <c r="C13" s="93"/>
       <c r="D13" s="93"/>
       <c r="E13" s="94" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F13" s="94"/>
       <c r="G13" s="94"/>
@@ -7665,15 +7593,15 @@
     </row>
     <row r="14" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" s="98" t="s">
         <v>181</v>
-      </c>
-      <c r="B14" s="98" t="s">
-        <v>182</v>
       </c>
       <c r="C14" s="98"/>
       <c r="D14" s="98"/>
       <c r="E14" s="94" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F14" s="94"/>
       <c r="G14" s="94"/>
@@ -7687,25 +7615,25 @@
       <c r="O14" s="94"/>
       <c r="P14" s="94"/>
       <c r="Q14" s="95" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="R14" s="95"/>
       <c r="S14" s="97" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T14" s="97"/>
     </row>
     <row r="15" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="92" t="s">
+        <v>184</v>
+      </c>
+      <c r="B15" s="93" t="s">
         <v>185</v>
-      </c>
-      <c r="B15" s="93" t="s">
-        <v>186</v>
       </c>
       <c r="C15" s="93"/>
       <c r="D15" s="93"/>
       <c r="E15" s="94" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F15" s="94"/>
       <c r="G15" s="94"/>
@@ -7725,15 +7653,15 @@
     </row>
     <row r="16" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="92" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="93" t="s">
         <v>188</v>
-      </c>
-      <c r="B16" s="93" t="s">
-        <v>189</v>
       </c>
       <c r="C16" s="93"/>
       <c r="D16" s="93"/>
       <c r="E16" s="94" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F16" s="94"/>
       <c r="G16" s="94"/>
@@ -7753,15 +7681,15 @@
     </row>
     <row r="17" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="92" t="s">
+        <v>190</v>
+      </c>
+      <c r="B17" s="93" t="s">
         <v>191</v>
-      </c>
-      <c r="B17" s="93" t="s">
-        <v>192</v>
       </c>
       <c r="C17" s="93"/>
       <c r="D17" s="93"/>
       <c r="E17" s="94" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F17" s="94"/>
       <c r="G17" s="94"/>
@@ -7777,21 +7705,21 @@
       <c r="Q17" s="95"/>
       <c r="R17" s="95"/>
       <c r="S17" s="97" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T17" s="97"/>
     </row>
     <row r="18" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="92" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="93" t="s">
         <v>195</v>
-      </c>
-      <c r="B18" s="93" t="s">
-        <v>196</v>
       </c>
       <c r="C18" s="93"/>
       <c r="D18" s="93"/>
       <c r="E18" s="94" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F18" s="94"/>
       <c r="G18" s="94"/>
@@ -7807,21 +7735,21 @@
       <c r="Q18" s="95"/>
       <c r="R18" s="95"/>
       <c r="S18" s="97" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T18" s="97"/>
     </row>
     <row r="19" customFormat="false" ht="33.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="92" t="s">
+        <v>198</v>
+      </c>
+      <c r="B19" s="99" t="s">
         <v>199</v>
-      </c>
-      <c r="B19" s="99" t="s">
-        <v>200</v>
       </c>
       <c r="C19" s="99"/>
       <c r="D19" s="99"/>
       <c r="E19" s="94" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F19" s="94"/>
       <c r="G19" s="94"/>
@@ -7841,15 +7769,15 @@
     </row>
     <row r="20" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="92" t="s">
+        <v>201</v>
+      </c>
+      <c r="B20" s="93" t="s">
         <v>202</v>
-      </c>
-      <c r="B20" s="93" t="s">
-        <v>203</v>
       </c>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
       <c r="E20" s="94" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F20" s="94"/>
       <c r="G20" s="94"/>
@@ -7865,21 +7793,21 @@
       <c r="Q20" s="95"/>
       <c r="R20" s="95"/>
       <c r="S20" s="97" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T20" s="97"/>
     </row>
     <row r="21" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="92" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" s="93" t="s">
         <v>205</v>
-      </c>
-      <c r="B21" s="93" t="s">
-        <v>206</v>
       </c>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
       <c r="E21" s="94" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F21" s="94"/>
       <c r="G21" s="94"/>
@@ -7899,15 +7827,15 @@
     </row>
     <row r="22" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="100" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" s="101" t="s">
         <v>208</v>
-      </c>
-      <c r="B22" s="101" t="s">
-        <v>209</v>
       </c>
       <c r="C22" s="101"/>
       <c r="D22" s="101"/>
       <c r="E22" s="94" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F22" s="94"/>
       <c r="G22" s="94"/>
@@ -7923,21 +7851,21 @@
       <c r="Q22" s="95"/>
       <c r="R22" s="95"/>
       <c r="S22" s="97" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T22" s="97"/>
     </row>
     <row r="23" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="102" t="s">
+        <v>210</v>
+      </c>
+      <c r="B23" s="103" t="s">
         <v>211</v>
-      </c>
-      <c r="B23" s="103" t="s">
-        <v>212</v>
       </c>
       <c r="C23" s="103"/>
       <c r="D23" s="103"/>
       <c r="E23" s="104" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F23" s="104"/>
       <c r="G23" s="104"/>
@@ -7979,7 +7907,7 @@
     </row>
     <row r="25" s="108" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="109" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B25" s="107"/>
       <c r="C25" s="107"/>
@@ -8003,7 +7931,7 @@
     </row>
     <row r="26" s="108" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="110" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B26" s="110"/>
       <c r="C26" s="110"/>
@@ -8049,7 +7977,7 @@
     </row>
     <row r="28" s="108" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="109" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B28" s="107"/>
       <c r="C28" s="107"/>
@@ -8073,7 +8001,7 @@
     </row>
     <row r="29" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="111" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B29" s="112" t="s">
         <v>52</v>
@@ -8082,10 +8010,10 @@
         <v>53</v>
       </c>
       <c r="D29" s="112" t="s">
+        <v>217</v>
+      </c>
+      <c r="E29" s="114" t="s">
         <v>218</v>
-      </c>
-      <c r="E29" s="114" t="s">
-        <v>219</v>
       </c>
       <c r="F29" s="115" t="s">
         <v>56</v>
@@ -8094,66 +8022,66 @@
         <v>57</v>
       </c>
       <c r="H29" s="112" t="s">
+        <v>219</v>
+      </c>
+      <c r="I29" s="116" t="s">
         <v>220</v>
       </c>
-      <c r="I29" s="116" t="s">
+      <c r="J29" s="114" t="s">
         <v>221</v>
       </c>
-      <c r="J29" s="114" t="s">
+      <c r="K29" s="115" t="s">
         <v>222</v>
       </c>
-      <c r="K29" s="115" t="s">
+      <c r="L29" s="116" t="s">
         <v>223</v>
       </c>
-      <c r="L29" s="116" t="s">
+      <c r="M29" s="113" t="s">
         <v>224</v>
       </c>
-      <c r="M29" s="113" t="s">
+      <c r="N29" s="117" t="s">
         <v>225</v>
       </c>
-      <c r="N29" s="117" t="s">
+      <c r="O29" s="115" t="s">
         <v>226</v>
       </c>
-      <c r="O29" s="115" t="s">
+      <c r="P29" s="113" t="s">
         <v>227</v>
       </c>
-      <c r="P29" s="113" t="s">
+      <c r="Q29" s="112" t="s">
         <v>228</v>
       </c>
-      <c r="Q29" s="112" t="s">
+      <c r="R29" s="114" t="s">
         <v>229</v>
       </c>
-      <c r="R29" s="114" t="s">
+      <c r="S29" s="118" t="s">
+        <v>208</v>
+      </c>
+      <c r="T29" s="119" t="s">
         <v>230</v>
-      </c>
-      <c r="S29" s="118" t="s">
-        <v>209</v>
-      </c>
-      <c r="T29" s="119" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="120" t="s">
+        <v>231</v>
+      </c>
+      <c r="B30" s="121" t="s">
         <v>232</v>
       </c>
-      <c r="B30" s="121" t="s">
+      <c r="C30" s="122" t="s">
         <v>233</v>
       </c>
-      <c r="C30" s="122" t="s">
+      <c r="D30" s="121" t="s">
         <v>234</v>
       </c>
-      <c r="D30" s="121" t="s">
+      <c r="E30" s="123" t="s">
         <v>235</v>
       </c>
-      <c r="E30" s="123" t="s">
+      <c r="F30" s="124" t="s">
         <v>236</v>
       </c>
-      <c r="F30" s="124" t="s">
+      <c r="G30" s="125" t="s">
         <v>237</v>
-      </c>
-      <c r="G30" s="125" t="s">
-        <v>238</v>
       </c>
       <c r="H30" s="126" t="n">
         <v>11000000</v>
@@ -8161,14 +8089,14 @@
       <c r="I30" s="127"/>
       <c r="J30" s="128"/>
       <c r="K30" s="121" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L30" s="129" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M30" s="130"/>
       <c r="N30" s="131" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O30" s="126" t="n">
         <v>81</v>
@@ -8179,29 +8107,29 @@
       </c>
       <c r="R30" s="123"/>
       <c r="S30" s="132" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="T30" s="133"/>
     </row>
     <row r="31" customFormat="false" ht="34.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="134" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B31" s="135" t="s">
+        <v>241</v>
+      </c>
+      <c r="C31" s="136" t="s">
         <v>242</v>
-      </c>
-      <c r="C31" s="136" t="s">
-        <v>243</v>
       </c>
       <c r="D31" s="137"/>
       <c r="E31" s="138" t="s">
+        <v>243</v>
+      </c>
+      <c r="F31" s="139" t="s">
         <v>244</v>
       </c>
-      <c r="F31" s="139" t="s">
+      <c r="G31" s="140" t="s">
         <v>245</v>
-      </c>
-      <c r="G31" s="140" t="s">
-        <v>246</v>
       </c>
       <c r="H31" s="141"/>
       <c r="I31" s="142" t="n">
@@ -8213,34 +8141,34 @@
       <c r="K31" s="137"/>
       <c r="L31" s="143"/>
       <c r="M31" s="136" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N31" s="144"/>
       <c r="O31" s="145"/>
       <c r="P31" s="136" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q31" s="137"/>
       <c r="R31" s="138" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="S31" s="146" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="T31" s="147"/>
     </row>
     <row r="32" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="148" t="s">
+        <v>248</v>
+      </c>
+      <c r="B32" s="149" t="s">
         <v>249</v>
       </c>
-      <c r="B32" s="149" t="s">
+      <c r="C32" s="150" t="s">
         <v>250</v>
       </c>
-      <c r="C32" s="150" t="s">
+      <c r="D32" s="151" t="s">
         <v>251</v>
-      </c>
-      <c r="D32" s="151" t="s">
-        <v>252</v>
       </c>
       <c r="E32" s="152"/>
       <c r="F32" s="153" t="n">
@@ -8258,7 +8186,7 @@
         <v>15</v>
       </c>
       <c r="L32" s="159" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M32" s="150"/>
       <c r="N32" s="160"/>
@@ -8266,22 +8194,22 @@
       <c r="P32" s="162"/>
       <c r="Q32" s="163"/>
       <c r="R32" s="164" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="S32" s="165"/>
       <c r="T32" s="166"/>
     </row>
     <row r="33" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="134" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B33" s="167" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C33" s="168"/>
       <c r="D33" s="169"/>
       <c r="E33" s="170" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F33" s="171" t="n">
         <v>42855</v>
@@ -8299,23 +8227,23 @@
       <c r="K33" s="174"/>
       <c r="L33" s="175"/>
       <c r="M33" s="176" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N33" s="177"/>
       <c r="O33" s="178"/>
       <c r="P33" s="179" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q33" s="180"/>
       <c r="R33" s="181" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="S33" s="182"/>
       <c r="T33" s="183"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="184" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B34" s="81"/>
       <c r="C34" s="185"/>
@@ -8361,7 +8289,7 @@
     </row>
     <row r="36" s="191" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="190" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B36" s="190"/>
       <c r="C36" s="190"/>
@@ -8385,7 +8313,7 @@
     </row>
     <row r="37" s="191" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="192" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B37" s="192"/>
       <c r="C37" s="192"/>
@@ -8409,7 +8337,7 @@
     </row>
     <row r="38" s="191" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="192" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B38" s="192"/>
       <c r="C38" s="192"/>
@@ -8433,7 +8361,7 @@
     </row>
     <row r="39" s="191" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="192" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B39" s="192"/>
       <c r="C39" s="192"/>
@@ -8457,7 +8385,7 @@
     </row>
     <row r="40" s="191" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="192" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B40" s="192"/>
       <c r="C40" s="192"/>
@@ -8481,7 +8409,7 @@
     </row>
     <row r="41" s="191" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="192" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B41" s="192"/>
       <c r="C41" s="192"/>
@@ -8505,7 +8433,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="193" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B42" s="193"/>
       <c r="C42" s="193"/>
@@ -8651,7 +8579,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="80" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -8679,7 +8607,7 @@
     </row>
     <row r="2" s="199" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="195" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2" s="196"/>
       <c r="C2" s="196"/>
@@ -8711,15 +8639,15 @@
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="83" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="84" t="s">
         <v>147</v>
-      </c>
-      <c r="B3" s="84" t="s">
-        <v>148</v>
       </c>
       <c r="C3" s="84"/>
       <c r="D3" s="84"/>
       <c r="E3" s="84" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F3" s="84"/>
       <c r="G3" s="84"/>
@@ -8733,34 +8661,34 @@
       <c r="O3" s="84"/>
       <c r="P3" s="84"/>
       <c r="Q3" s="85" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="R3" s="85"/>
       <c r="S3" s="85" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="T3" s="85"/>
       <c r="U3" s="85" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="V3" s="85"/>
       <c r="W3" s="86" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="X3" s="86"/>
       <c r="Y3" s="200"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="201" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="202" t="s">
         <v>152</v>
-      </c>
-      <c r="B4" s="202" t="s">
-        <v>153</v>
       </c>
       <c r="C4" s="202"/>
       <c r="D4" s="202"/>
       <c r="E4" s="89" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F4" s="89"/>
       <c r="G4" s="89"/>
@@ -8774,34 +8702,34 @@
       <c r="O4" s="89"/>
       <c r="P4" s="89"/>
       <c r="Q4" s="203" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R4" s="203"/>
       <c r="S4" s="203" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T4" s="203"/>
       <c r="U4" s="203" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V4" s="203"/>
       <c r="W4" s="96" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X4" s="96"/>
       <c r="Y4" s="200"/>
     </row>
     <row r="5" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="93" t="s">
         <v>156</v>
-      </c>
-      <c r="B5" s="93" t="s">
-        <v>157</v>
       </c>
       <c r="C5" s="93"/>
       <c r="D5" s="93"/>
       <c r="E5" s="94" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F5" s="94"/>
       <c r="G5" s="94"/>
@@ -8819,7 +8747,7 @@
       <c r="S5" s="95"/>
       <c r="T5" s="95"/>
       <c r="U5" s="95" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V5" s="95"/>
       <c r="W5" s="97"/>
@@ -8828,15 +8756,15 @@
     </row>
     <row r="6" customFormat="false" ht="110.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="92" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" s="93" t="s">
         <v>159</v>
-      </c>
-      <c r="B6" s="93" t="s">
-        <v>160</v>
       </c>
       <c r="C6" s="93"/>
       <c r="D6" s="93"/>
       <c r="E6" s="94" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F6" s="94"/>
       <c r="G6" s="94"/>
@@ -8850,34 +8778,34 @@
       <c r="O6" s="94"/>
       <c r="P6" s="94"/>
       <c r="Q6" s="95" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R6" s="95"/>
       <c r="S6" s="95" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="T6" s="95"/>
       <c r="U6" s="95" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="V6" s="95"/>
       <c r="W6" s="204" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="X6" s="204"/>
       <c r="Y6" s="200"/>
     </row>
     <row r="7" customFormat="false" ht="110.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="92" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="93" t="s">
         <v>163</v>
-      </c>
-      <c r="B7" s="93" t="s">
-        <v>164</v>
       </c>
       <c r="C7" s="93"/>
       <c r="D7" s="93"/>
       <c r="E7" s="94" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F7" s="94"/>
       <c r="G7" s="94"/>
@@ -8902,15 +8830,15 @@
     </row>
     <row r="8" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="92" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="93" t="s">
         <v>166</v>
-      </c>
-      <c r="B8" s="93" t="s">
-        <v>167</v>
       </c>
       <c r="C8" s="93"/>
       <c r="D8" s="93"/>
       <c r="E8" s="94" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F8" s="94"/>
       <c r="G8" s="94"/>
@@ -8924,24 +8852,24 @@
       <c r="O8" s="94"/>
       <c r="P8" s="94"/>
       <c r="Q8" s="95" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R8" s="95"/>
       <c r="S8" s="95"/>
       <c r="T8" s="95"/>
       <c r="U8" s="95" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V8" s="95"/>
       <c r="W8" s="97" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X8" s="97"/>
       <c r="Y8" s="200"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="92" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="93" t="s">
         <v>57</v>
@@ -8949,7 +8877,7 @@
       <c r="C9" s="93"/>
       <c r="D9" s="93"/>
       <c r="E9" s="94" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F9" s="94"/>
       <c r="G9" s="94"/>
@@ -8965,7 +8893,7 @@
       <c r="Q9" s="95"/>
       <c r="R9" s="95"/>
       <c r="S9" s="95" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T9" s="95"/>
       <c r="U9" s="95"/>
@@ -8976,15 +8904,15 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="92" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="93" t="s">
         <v>171</v>
-      </c>
-      <c r="B10" s="93" t="s">
-        <v>172</v>
       </c>
       <c r="C10" s="93"/>
       <c r="D10" s="93"/>
       <c r="E10" s="94" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F10" s="94"/>
       <c r="G10" s="94"/>
@@ -9000,11 +8928,11 @@
       <c r="Q10" s="95"/>
       <c r="R10" s="95"/>
       <c r="S10" s="95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T10" s="95"/>
       <c r="U10" s="95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="V10" s="95"/>
       <c r="W10" s="97"/>
@@ -9013,15 +8941,15 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="92" t="s">
+        <v>174</v>
+      </c>
+      <c r="B11" s="93" t="s">
         <v>175</v>
-      </c>
-      <c r="B11" s="93" t="s">
-        <v>176</v>
       </c>
       <c r="C11" s="93"/>
       <c r="D11" s="93"/>
       <c r="E11" s="94" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F11" s="94"/>
       <c r="G11" s="94"/>
@@ -9046,15 +8974,15 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="93" t="s">
         <v>178</v>
-      </c>
-      <c r="B12" s="93" t="s">
-        <v>179</v>
       </c>
       <c r="C12" s="93"/>
       <c r="D12" s="93"/>
       <c r="E12" s="94" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F12" s="94"/>
       <c r="G12" s="94"/>
@@ -9079,15 +9007,15 @@
     </row>
     <row r="13" customFormat="false" ht="68.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="98" t="s">
         <v>181</v>
-      </c>
-      <c r="B13" s="98" t="s">
-        <v>182</v>
       </c>
       <c r="C13" s="98"/>
       <c r="D13" s="98"/>
       <c r="E13" s="94" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F13" s="94"/>
       <c r="G13" s="94"/>
@@ -9101,34 +9029,34 @@
       <c r="O13" s="94"/>
       <c r="P13" s="94"/>
       <c r="Q13" s="95" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="R13" s="95"/>
       <c r="S13" s="95" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T13" s="95"/>
       <c r="U13" s="95" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V13" s="95"/>
       <c r="W13" s="97" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="X13" s="97"/>
       <c r="Y13" s="200"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="92" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="93" t="s">
         <v>185</v>
-      </c>
-      <c r="B14" s="93" t="s">
-        <v>186</v>
       </c>
       <c r="C14" s="93"/>
       <c r="D14" s="93"/>
       <c r="E14" s="94" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F14" s="94"/>
       <c r="G14" s="94"/>
@@ -9153,15 +9081,15 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="92" t="s">
+        <v>187</v>
+      </c>
+      <c r="B15" s="93" t="s">
         <v>188</v>
-      </c>
-      <c r="B15" s="93" t="s">
-        <v>189</v>
       </c>
       <c r="C15" s="93"/>
       <c r="D15" s="93"/>
       <c r="E15" s="94" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F15" s="94"/>
       <c r="G15" s="94"/>
@@ -9186,15 +9114,15 @@
     </row>
     <row r="16" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="92" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" s="93" t="s">
         <v>191</v>
-      </c>
-      <c r="B16" s="93" t="s">
-        <v>192</v>
       </c>
       <c r="C16" s="93"/>
       <c r="D16" s="93"/>
       <c r="E16" s="94" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F16" s="94"/>
       <c r="G16" s="94"/>
@@ -9219,15 +9147,15 @@
     </row>
     <row r="17" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="92" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="93" t="s">
         <v>195</v>
-      </c>
-      <c r="B17" s="93" t="s">
-        <v>196</v>
       </c>
       <c r="C17" s="93"/>
       <c r="D17" s="93"/>
       <c r="E17" s="94" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F17" s="94"/>
       <c r="G17" s="94"/>
@@ -9241,34 +9169,34 @@
       <c r="O17" s="94"/>
       <c r="P17" s="94"/>
       <c r="Q17" s="94" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="R17" s="94"/>
       <c r="S17" s="95" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T17" s="95"/>
       <c r="U17" s="95" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="V17" s="95"/>
       <c r="W17" s="204" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="X17" s="204"/>
       <c r="Y17" s="200"/>
     </row>
     <row r="18" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="92" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" s="99" t="s">
         <v>199</v>
-      </c>
-      <c r="B18" s="99" t="s">
-        <v>200</v>
       </c>
       <c r="C18" s="99"/>
       <c r="D18" s="99"/>
       <c r="E18" s="94" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F18" s="94"/>
       <c r="G18" s="94"/>
@@ -9293,15 +9221,15 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="92" t="s">
+        <v>201</v>
+      </c>
+      <c r="B19" s="93" t="s">
         <v>202</v>
-      </c>
-      <c r="B19" s="93" t="s">
-        <v>203</v>
       </c>
       <c r="C19" s="93"/>
       <c r="D19" s="93"/>
       <c r="E19" s="94" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F19" s="94"/>
       <c r="G19" s="94"/>
@@ -9319,7 +9247,7 @@
       <c r="S19" s="95"/>
       <c r="T19" s="95"/>
       <c r="U19" s="95" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="V19" s="95"/>
       <c r="W19" s="97"/>
@@ -9328,15 +9256,15 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="92" t="s">
+        <v>204</v>
+      </c>
+      <c r="B20" s="93" t="s">
         <v>205</v>
-      </c>
-      <c r="B20" s="93" t="s">
-        <v>206</v>
       </c>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
       <c r="E20" s="94" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F20" s="94"/>
       <c r="G20" s="94"/>
@@ -9361,15 +9289,15 @@
     </row>
     <row r="21" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="100" t="s">
+        <v>207</v>
+      </c>
+      <c r="B21" s="101" t="s">
         <v>208</v>
-      </c>
-      <c r="B21" s="101" t="s">
-        <v>209</v>
       </c>
       <c r="C21" s="101"/>
       <c r="D21" s="101"/>
       <c r="E21" s="94" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F21" s="94"/>
       <c r="G21" s="94"/>
@@ -9394,15 +9322,15 @@
     </row>
     <row r="22" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="102" t="s">
+        <v>210</v>
+      </c>
+      <c r="B22" s="103" t="s">
         <v>211</v>
-      </c>
-      <c r="B22" s="103" t="s">
-        <v>212</v>
       </c>
       <c r="C22" s="103"/>
       <c r="D22" s="103"/>
       <c r="E22" s="104" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F22" s="104"/>
       <c r="G22" s="104"/>
@@ -9430,7 +9358,7 @@
     </row>
     <row r="23" s="193" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="207" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B23" s="207"/>
       <c r="C23" s="207"/>

</xml_diff>